<commit_message>
last changes by running ablation analysis
</commit_message>
<xml_diff>
--- a/data/correlation_analysis_intepretation_timeout_max.xlsx
+++ b/data/correlation_analysis_intepretation_timeout_max.xlsx
@@ -8,23 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ojcchar/repositories/Projects/complexity-verification-project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B32D96C-2815-544B-BD47-E205EAF3F571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781045F3-BD2F-B143-977A-2B5620562A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="760" windowWidth="30240" windowHeight="17680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_tools" sheetId="1" r:id="rId1"/>
-    <sheet name="checker_framework" sheetId="2" r:id="rId2"/>
-    <sheet name="typestate_checker" sheetId="3" r:id="rId3"/>
-    <sheet name="infer" sheetId="4" r:id="rId4"/>
-    <sheet name="openjml" sheetId="5" r:id="rId5"/>
+    <sheet name="all_but_chck_frm" sheetId="6" r:id="rId2"/>
+    <sheet name="checker_framework" sheetId="2" r:id="rId3"/>
+    <sheet name="typestate_checker" sheetId="3" r:id="rId4"/>
+    <sheet name="infer" sheetId="4" r:id="rId5"/>
+    <sheet name="openjml" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">all_but_chck_frm!$A$1:$O$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_tools!$A$1:$O$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">checker_framework!$A$1:$O$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">infer!$A$1:$O$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">openjml!$A$1:$O$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">typestate_checker!$A$1:$O$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">checker_framework!$A$1:$O$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">infer!$A$1:$O$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">openjml!$A$1:$O$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">typestate_checker!$A$1:$O$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="59">
   <si>
     <t>metric</t>
   </si>
@@ -362,7 +364,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -446,6 +448,45 @@
     <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,11 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M20"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1253,25 +1293,25 @@
         <v>100</v>
       </c>
       <c r="F9" s="11">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G9" s="11">
-        <v>829</v>
+        <v>1200</v>
       </c>
       <c r="H9" s="11">
         <v>100</v>
       </c>
       <c r="I9" s="41">
-        <v>-0.24781837462692349</v>
+        <v>-0.16799308498171919</v>
       </c>
       <c r="J9" s="11">
-        <v>3.7575890366249538E-4</v>
+        <v>1.571209940531982E-2</v>
       </c>
       <c r="K9" s="11">
-        <v>-0.37848331556821152</v>
+        <v>-0.25815625942948522</v>
       </c>
       <c r="L9" s="11">
-        <v>1.032931167420872E-4</v>
+        <v>9.5081814155965165E-3</v>
       </c>
       <c r="M9" s="26" t="str">
         <f t="shared" si="0"/>
@@ -1283,7 +1323,7 @@
       </c>
       <c r="O9" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>**</v>
+        <v>*</v>
       </c>
       <c r="Q9" s="36">
         <v>0.3</v>
@@ -1315,7 +1355,7 @@
         <v>48</v>
       </c>
       <c r="G10" s="14">
-        <v>903</v>
+        <v>863</v>
       </c>
       <c r="H10" s="14">
         <v>50</v>
@@ -1374,7 +1414,7 @@
         <v>48</v>
       </c>
       <c r="G11" s="14">
-        <v>903</v>
+        <v>863</v>
       </c>
       <c r="H11" s="14">
         <v>50</v>
@@ -1404,7 +1444,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:19" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>18</v>
       </c>
@@ -1424,7 +1464,7 @@
         <v>48</v>
       </c>
       <c r="G12" s="14">
-        <v>903</v>
+        <v>863</v>
       </c>
       <c r="H12" s="14">
         <v>50</v>
@@ -1504,7 +1544,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:19" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>24</v>
       </c>
@@ -1554,7 +1594,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:19" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>23</v>
       </c>
@@ -1604,7 +1644,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:19" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>25</v>
       </c>
@@ -1854,7 +1894,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:15" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>18</v>
       </c>
@@ -1977,27 +2017,1291 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O21" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="12">
-      <filters>
-        <filter val="y"/>
-      </filters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O21">
-      <sortCondition ref="B1:B21"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:O21" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E939B00-1BCE-E144-83FE-38E5D5F3CE22}">
+  <dimension ref="A1:S30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="21.6640625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="8.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="5">
+        <v>23</v>
+      </c>
+      <c r="I2" s="39">
+        <v>-0.34743961448615102</v>
+      </c>
+      <c r="J2" s="5">
+        <v>3.2806356472939502E-2</v>
+      </c>
+      <c r="K2" s="5">
+        <v>-0.27197235029387162</v>
+      </c>
+      <c r="L2" s="5">
+        <v>0.20932509565963231</v>
+      </c>
+      <c r="M2" s="22" t="str">
+        <f t="shared" ref="M2:M21" si="0">IF(ISBLANK(I2),"",IF(AND(D2="negative",I2&lt;0),"y",IF(AND(D2="positive",I2&gt;0), "y","n")))</f>
+        <v>y</v>
+      </c>
+      <c r="N2" s="23" t="str">
+        <f>IF(ISBLANK(I2),"",LOOKUP(ABS(I2),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
+        <v>Medium</v>
+      </c>
+      <c r="O2" s="23" t="str">
+        <f t="shared" ref="O2:O3" si="1">IF(ISBLANK(I2),"",IF(J2&lt;0.01,"**",IF(J2&lt;0.05,"*", "")))</f>
+        <v>*</v>
+      </c>
+      <c r="P2" s="6" t="str">
+        <f>IF(ABS(I2)&gt;ABS(all_tools!I2),"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="Q2" s="6" t="str">
+        <f>IF(ABS(I2)&lt;ABS(all_tools!I2),"y","")</f>
+        <v/>
+      </c>
+      <c r="R2" s="6" t="str">
+        <f>IF(M2=all_tools!M2,"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="S2" s="49">
+        <f>ABS(I2)-ABS(all_tools!I2)</f>
+        <v>9.71186674312563E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="5">
+        <v>23</v>
+      </c>
+      <c r="I3" s="39">
+        <v>-0.45043061778919702</v>
+      </c>
+      <c r="J3" s="5">
+        <v>5.0370573016936798E-3</v>
+      </c>
+      <c r="K3" s="5">
+        <v>-0.32017787305285961</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0.13637641008504059</v>
+      </c>
+      <c r="M3" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>y</v>
+      </c>
+      <c r="N3" s="23" t="str">
+        <f>IF(ISBLANK(I3),"",LOOKUP(ABS(I3),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
+        <v>Medium</v>
+      </c>
+      <c r="O3" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>**</v>
+      </c>
+      <c r="P3" s="6" t="str">
+        <f>IF(ABS(I3)&gt;ABS(all_tools!I3),"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="Q3" s="6" t="str">
+        <f>IF(ABS(I3)&lt;ABS(all_tools!I3),"y","")</f>
+        <v/>
+      </c>
+      <c r="R3" s="6" t="str">
+        <f>IF(M3=all_tools!M3,"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="S3" s="49">
+        <f>ABS(I3)-ABS(all_tools!I3)</f>
+        <v>2.2882327096323207E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="5">
+        <v>23</v>
+      </c>
+      <c r="I4" s="39">
+        <v>0.433840500094132</v>
+      </c>
+      <c r="J4" s="5">
+        <v>6.5485311386563796E-3</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0.28096954242303013</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0.19405167261558409</v>
+      </c>
+      <c r="M4" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>y</v>
+      </c>
+      <c r="N4" s="23" t="str">
+        <f>IF(ISBLANK(I4),"",LOOKUP(ABS(I4),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
+        <v>Medium</v>
+      </c>
+      <c r="O4" s="23" t="str">
+        <f>IF(ISBLANK(I4),"",IF(J4&lt;0.01,"**",IF(J4&lt;0.05,"*", "")))</f>
+        <v>**</v>
+      </c>
+      <c r="P4" s="6" t="str">
+        <f>IF(ABS(I4)&gt;ABS(all_tools!I4),"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="Q4" s="6" t="str">
+        <f>IF(ABS(I4)&lt;ABS(all_tools!I4),"y","")</f>
+        <v/>
+      </c>
+      <c r="R4" s="6" t="str">
+        <f>IF(M4=all_tools!M4,"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="S4" s="49">
+        <f>ABS(I4)-ABS(all_tools!I4)</f>
+        <v>2.2669840083568205E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="8">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="7">
+        <v>12</v>
+      </c>
+      <c r="I5" s="40">
+        <v>-0.31333978072025598</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.188469990901005</v>
+      </c>
+      <c r="M5" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>y</v>
+      </c>
+      <c r="N5" s="25" t="str">
+        <f>IF(ISBLANK(I5),"",LOOKUP(ABS(I5),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
+        <v>Medium</v>
+      </c>
+      <c r="O5" s="25" t="str">
+        <f t="shared" ref="O5:O21" si="2">IF(ISBLANK(I5),"",IF(J5&lt;0.01,"**",IF(J5&lt;0.05,"*", "")))</f>
+        <v/>
+      </c>
+      <c r="P5" s="8" t="str">
+        <f>IF(ABS(I5)&gt;ABS(all_tools!I5),"y","")</f>
+        <v/>
+      </c>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8" t="str">
+        <f>IF(M5=all_tools!M5,"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="S5" s="50">
+        <f>ABS(I5)-ABS(all_tools!I5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="8">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="7">
+        <v>12</v>
+      </c>
+      <c r="I6" s="40">
+        <v>-0.45260190548481399</v>
+      </c>
+      <c r="J6" s="7">
+        <v>5.7483531731336301E-2</v>
+      </c>
+      <c r="M6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>y</v>
+      </c>
+      <c r="N6" s="25" t="str">
+        <f>IF(ISBLANK(I6),"",LOOKUP(ABS(I6),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
+        <v>Medium</v>
+      </c>
+      <c r="O6" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P6" s="8" t="str">
+        <f>IF(ABS(I6)&gt;ABS(all_tools!I6),"y","")</f>
+        <v/>
+      </c>
+      <c r="Q6" s="51"/>
+      <c r="R6" s="51" t="str">
+        <f>IF(M6=all_tools!M6,"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="S6" s="52">
+        <f>ABS(I6)-ABS(all_tools!I6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="8">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="7">
+        <v>12</v>
+      </c>
+      <c r="I7" s="40">
+        <v>-0.38297084310253499</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0.107973801457466</v>
+      </c>
+      <c r="M7" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>y</v>
+      </c>
+      <c r="N7" s="25" t="str">
+        <f>IF(ISBLANK(I7),"",LOOKUP(ABS(I7),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
+        <v>Medium</v>
+      </c>
+      <c r="O7" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P7" s="8" t="str">
+        <f>IF(ABS(I7)&gt;ABS(all_tools!I7),"y","")</f>
+        <v/>
+      </c>
+      <c r="Q7" s="53"/>
+      <c r="R7" s="53" t="str">
+        <f>IF(M7=all_tools!M7,"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="S7" s="54">
+        <f>ABS(I7)-ABS(all_tools!I7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="7">
+        <v>12</v>
+      </c>
+      <c r="I8" s="40">
+        <v>0.13926212476455799</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0.55888582904161999</v>
+      </c>
+      <c r="M8" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>y</v>
+      </c>
+      <c r="N8" s="25" t="str">
+        <f>IF(ISBLANK(I8),"",LOOKUP(ABS(I8),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
+        <v>Small</v>
+      </c>
+      <c r="O8" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P8" s="8" t="str">
+        <f>IF(ABS(I8)&gt;ABS(all_tools!I8),"y","")</f>
+        <v/>
+      </c>
+      <c r="Q8" s="53"/>
+      <c r="R8" s="53" t="str">
+        <f>IF(M8=all_tools!M8,"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="S8" s="54">
+        <f>ABS(I8)-ABS(all_tools!I8)</f>
+        <v>-3.0531133177191805E-16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="12">
+        <v>3</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="11">
+        <v>100</v>
+      </c>
+      <c r="I9" s="41">
+        <v>-0.151284214661567</v>
+      </c>
+      <c r="J9" s="11">
+        <v>2.9534236432747201E-2</v>
+      </c>
+      <c r="K9" s="11">
+        <v>-0.28726717466178431</v>
+      </c>
+      <c r="L9" s="11">
+        <v>3.7567205497513649E-3</v>
+      </c>
+      <c r="M9" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>y</v>
+      </c>
+      <c r="N9" s="27" t="str">
+        <f>IF(ISBLANK(I9),"",LOOKUP(ABS(I9),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
+        <v>Small</v>
+      </c>
+      <c r="O9" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v>*</v>
+      </c>
+      <c r="P9" s="12" t="str">
+        <f>IF(ABS(I9)&gt;ABS(all_tools!I9),"y","")</f>
+        <v/>
+      </c>
+      <c r="Q9" s="55" t="str">
+        <f>IF(ABS(I9)&lt;ABS(all_tools!I9),"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="R9" s="55" t="str">
+        <f>IF(M9=all_tools!M9,"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="S9" s="56">
+        <f>ABS(I9)-ABS(all_tools!I9)</f>
+        <v>-1.6708870320152197E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="15">
+        <v>6</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="14">
+        <v>50</v>
+      </c>
+      <c r="I10" s="42">
+        <v>-1.7889603976091299E-2</v>
+      </c>
+      <c r="J10" s="14">
+        <v>0.88317001415190299</v>
+      </c>
+      <c r="K10" s="14">
+        <v>-2.1745521452022229E-2</v>
+      </c>
+      <c r="L10" s="14">
+        <v>0.88084937555910936</v>
+      </c>
+      <c r="M10" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>y</v>
+      </c>
+      <c r="N10" s="29" t="str">
+        <f>IF(ISBLANK(I10),"",LOOKUP(ABS(I10),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
+        <v>None</v>
+      </c>
+      <c r="O10" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P10" s="15" t="str">
+        <f>IF(ABS(I10)&gt;ABS(all_tools!I10),"y","")</f>
+        <v/>
+      </c>
+      <c r="Q10" s="57" t="str">
+        <f>IF(ABS(I10)&lt;ABS(all_tools!I10),"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="R10" s="57" t="str">
+        <f>IF(M10=all_tools!M10,"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="S10" s="58">
+        <f>ABS(I10)-ABS(all_tools!I10)</f>
+        <v>-5.2041704279304213E-17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="15">
+        <v>6</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="14">
+        <v>50</v>
+      </c>
+      <c r="I11" s="42">
+        <v>-3.1906673122880098E-2</v>
+      </c>
+      <c r="J11" s="14">
+        <v>0.78376723002502102</v>
+      </c>
+      <c r="K11" s="14">
+        <v>-2.8051607294758089E-2</v>
+      </c>
+      <c r="L11" s="14">
+        <v>0.84666464123863983</v>
+      </c>
+      <c r="M11" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>y</v>
+      </c>
+      <c r="N11" s="29" t="str">
+        <f>IF(ISBLANK(I11),"",LOOKUP(ABS(I11),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
+        <v>None</v>
+      </c>
+      <c r="O11" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P11" s="15" t="str">
+        <f>IF(ABS(I11)&gt;ABS(all_tools!I11),"y","")</f>
+        <v/>
+      </c>
+      <c r="Q11" s="15" t="str">
+        <f>IF(ABS(I11)&lt;ABS(all_tools!I11),"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="R11" s="15" t="str">
+        <f>IF(M11=all_tools!M11,"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="S11" s="59">
+        <f>ABS(I11)-ABS(all_tools!I11)</f>
+        <v>-1.0408340855860843E-16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="15">
+        <v>6</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="14">
+        <v>50</v>
+      </c>
+      <c r="I12" s="42">
+        <v>-0.244157078771431</v>
+      </c>
+      <c r="J12" s="14">
+        <v>3.4554165539190197E-2</v>
+      </c>
+      <c r="K12" s="14">
+        <v>-0.31183200892839741</v>
+      </c>
+      <c r="L12" s="14">
+        <v>2.7488825966879269E-2</v>
+      </c>
+      <c r="M12" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+      <c r="N12" s="29" t="str">
+        <f>IF(ISBLANK(I12),"",LOOKUP(ABS(I12),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
+        <v>Small</v>
+      </c>
+      <c r="O12" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v>*</v>
+      </c>
+      <c r="P12" s="15" t="str">
+        <f>IF(ABS(I12)&gt;ABS(all_tools!I12),"y","")</f>
+        <v/>
+      </c>
+      <c r="Q12" s="15" t="str">
+        <f>IF(ABS(I12)&lt;ABS(all_tools!I12),"y","")</f>
+        <v/>
+      </c>
+      <c r="R12" s="15" t="str">
+        <f>IF(M12=all_tools!M12,"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="S12" s="59">
+        <f>ABS(I12)-ABS(all_tools!I12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="17">
+        <v>10</v>
+      </c>
+      <c r="I13" s="43">
+        <v>-0.31859300290731601</v>
+      </c>
+      <c r="J13" s="17">
+        <v>0.224066686312096</v>
+      </c>
+      <c r="K13" s="17">
+        <v>-0.42640143271122077</v>
+      </c>
+      <c r="L13" s="17">
+        <v>0.21913836052287261</v>
+      </c>
+      <c r="M13" s="30" t="str">
+        <f t="shared" si="0"/>
+        <v>y</v>
+      </c>
+      <c r="N13" s="31" t="str">
+        <f>IF(ISBLANK(I13),"",LOOKUP(ABS(I13),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
+        <v>Medium</v>
+      </c>
+      <c r="O13" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P13" s="18" t="str">
+        <f>IF(ABS(I13)&gt;ABS(all_tools!I13),"y","")</f>
+        <v/>
+      </c>
+      <c r="Q13" s="18" t="str">
+        <f>IF(ABS(I13)&lt;ABS(all_tools!I13),"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="R13" s="18" t="str">
+        <f>IF(M13=all_tools!M13,"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="S13" s="60">
+        <f>ABS(I13)-ABS(all_tools!I13)</f>
+        <v>-0.13494641731765816</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="17">
+        <v>10</v>
+      </c>
+      <c r="I14" s="43">
+        <v>0.171550078488555</v>
+      </c>
+      <c r="J14" s="17">
+        <v>0.51269076026192295</v>
+      </c>
+      <c r="K14" s="17">
+        <v>0.35533452725935072</v>
+      </c>
+      <c r="L14" s="17">
+        <v>0.31363736407545367</v>
+      </c>
+      <c r="M14" s="30" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+      <c r="N14" s="31" t="str">
+        <f>IF(ISBLANK(I14),"",LOOKUP(ABS(I14),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
+        <v>Small</v>
+      </c>
+      <c r="O14" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P14" s="18" t="str">
+        <f>IF(ABS(I14)&gt;ABS(all_tools!I14),"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="Q14" s="18" t="str">
+        <f>IF(ABS(I14)&lt;ABS(all_tools!I14),"y","")</f>
+        <v/>
+      </c>
+      <c r="R14" s="18" t="str">
+        <f>IF(M14=all_tools!M14,"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="S14" s="60">
+        <f>ABS(I14)-ABS(all_tools!I14)</f>
+        <v>5.2197599481982895E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="17">
+        <v>10</v>
+      </c>
+      <c r="I15" s="43">
+        <v>0.171550078488555</v>
+      </c>
+      <c r="J15" s="17">
+        <v>0.51269076026192295</v>
+      </c>
+      <c r="K15" s="17">
+        <v>0.42640143271122077</v>
+      </c>
+      <c r="L15" s="17">
+        <v>0.21913836052287261</v>
+      </c>
+      <c r="M15" s="30" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+      <c r="N15" s="31" t="str">
+        <f>IF(ISBLANK(I15),"",LOOKUP(ABS(I15),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
+        <v>Small</v>
+      </c>
+      <c r="O15" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P15" s="18" t="str">
+        <f>IF(ABS(I15)&gt;ABS(all_tools!I15),"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="Q15" s="18" t="str">
+        <f>IF(ABS(I15)&lt;ABS(all_tools!I15),"y","")</f>
+        <v/>
+      </c>
+      <c r="R15" s="18" t="str">
+        <f>IF(M15=all_tools!M15,"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="S15" s="60">
+        <f>ABS(I15)-ABS(all_tools!I15)</f>
+        <v>4.4566078793540076E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="17">
+        <v>10</v>
+      </c>
+      <c r="I16" s="43">
+        <v>-0.269578694767729</v>
+      </c>
+      <c r="J16" s="17">
+        <v>0.30360117123335201</v>
+      </c>
+      <c r="K16" s="17">
+        <v>-0.497468338163091</v>
+      </c>
+      <c r="L16" s="17">
+        <v>0.14346146559508571</v>
+      </c>
+      <c r="M16" s="30" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+      <c r="N16" s="31" t="str">
+        <f>IF(ISBLANK(I16),"",LOOKUP(ABS(I16),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
+        <v>Small</v>
+      </c>
+      <c r="O16" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P16" s="18" t="str">
+        <f>IF(ABS(I16)&gt;ABS(all_tools!I16),"y","")</f>
+        <v/>
+      </c>
+      <c r="Q16" s="18" t="str">
+        <f>IF(ABS(I16)&lt;ABS(all_tools!I16),"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="R16" s="18" t="str">
+        <f>IF(M16=all_tools!M16,"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="S16" s="60">
+        <f>ABS(I16)-ABS(all_tools!I16)</f>
+        <v>-8.8478742251987375E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="19">
+        <v>16</v>
+      </c>
+      <c r="I17" s="44">
+        <v>-0.109544511501033</v>
+      </c>
+      <c r="J17" s="19">
+        <v>0.57719497655386198</v>
+      </c>
+      <c r="K17" s="19">
+        <v>-0.12157835800107809</v>
+      </c>
+      <c r="L17" s="19">
+        <v>0.65376710935384819</v>
+      </c>
+      <c r="M17" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>y</v>
+      </c>
+      <c r="N17" s="33" t="str">
+        <f>IF(ISBLANK(I17),"",LOOKUP(ABS(I17),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
+        <v>Small</v>
+      </c>
+      <c r="O17" s="33" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P17" s="20" t="str">
+        <f>IF(ABS(I17)&gt;ABS(all_tools!I17),"y","")</f>
+        <v/>
+      </c>
+      <c r="Q17" s="20" t="str">
+        <f>IF(ABS(I17)&lt;ABS(all_tools!I17),"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="R17" s="20" t="str">
+        <f>IF(M17=all_tools!M17,"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="S17" s="61">
+        <f>ABS(I17)-ABS(all_tools!I17)</f>
+        <v>-7.1230870014513809E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="19">
+        <v>16</v>
+      </c>
+      <c r="I18" s="44">
+        <v>-0.14605934866804399</v>
+      </c>
+      <c r="J18" s="19">
+        <v>0.457290667956682</v>
+      </c>
+      <c r="K18" s="19">
+        <v>-1.736833685729687E-2</v>
+      </c>
+      <c r="L18" s="19">
+        <v>0.94909603273704102</v>
+      </c>
+      <c r="M18" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>y</v>
+      </c>
+      <c r="N18" s="33" t="str">
+        <f>IF(ISBLANK(I18),"",LOOKUP(ABS(I18),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
+        <v>Small</v>
+      </c>
+      <c r="O18" s="33" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P18" s="20" t="str">
+        <f>IF(ABS(I18)&gt;ABS(all_tools!I18),"y","")</f>
+        <v/>
+      </c>
+      <c r="Q18" s="20" t="str">
+        <f>IF(ABS(I18)&lt;ABS(all_tools!I18),"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="R18" s="20" t="str">
+        <f>IF(M18=all_tools!M18,"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="S18" s="61">
+        <f>ABS(I18)-ABS(all_tools!I18)</f>
+        <v>-3.4716032847502826E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="19">
+        <v>16</v>
+      </c>
+      <c r="I19" s="44">
+        <v>0.30251050401930901</v>
+      </c>
+      <c r="J19" s="19">
+        <v>0.124914355449184</v>
+      </c>
+      <c r="K19" s="19">
+        <v>0.3302413141237342</v>
+      </c>
+      <c r="L19" s="19">
+        <v>0.21158246186830859</v>
+      </c>
+      <c r="M19" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>y</v>
+      </c>
+      <c r="N19" s="33" t="str">
+        <f>IF(ISBLANK(I19),"",LOOKUP(ABS(I19),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
+        <v>Medium</v>
+      </c>
+      <c r="O19" s="33" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P19" s="20" t="str">
+        <f>IF(ABS(I19)&gt;ABS(all_tools!I19),"y","")</f>
+        <v/>
+      </c>
+      <c r="Q19" s="20" t="str">
+        <f>IF(ABS(I19)&lt;ABS(all_tools!I19),"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="R19" s="20" t="str">
+        <f>IF(M19=all_tools!M19,"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="S19" s="61">
+        <f>ABS(I19)-ABS(all_tools!I19)</f>
+        <v>-5.1479534129019511E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="19">
+        <v>16</v>
+      </c>
+      <c r="I20" s="44">
+        <v>-0.16641005886756799</v>
+      </c>
+      <c r="J20" s="19">
+        <v>0.40142102402695501</v>
+      </c>
+      <c r="K20" s="19">
+        <v>-0.19161611347062391</v>
+      </c>
+      <c r="L20" s="19">
+        <v>0.4771333722542902</v>
+      </c>
+      <c r="M20" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>y</v>
+      </c>
+      <c r="N20" s="33" t="str">
+        <f>IF(ISBLANK(I20),"",LOOKUP(ABS(I20),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
+        <v>Small</v>
+      </c>
+      <c r="O20" s="33" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P20" s="20" t="str">
+        <f>IF(ABS(I20)&gt;ABS(all_tools!I20),"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="Q20" s="20" t="str">
+        <f>IF(ABS(I20)&lt;ABS(all_tools!I20),"y","")</f>
+        <v/>
+      </c>
+      <c r="R20" s="20" t="str">
+        <f>IF(M20=all_tools!M20,"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="S20" s="61">
+        <f>ABS(I20)-ABS(all_tools!I20)</f>
+        <v>1.6395479532410884E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" s="19">
+        <v>16</v>
+      </c>
+      <c r="I21" s="44">
+        <v>-9.1287092917527596E-2</v>
+      </c>
+      <c r="J21" s="19">
+        <v>0.642237837292436</v>
+      </c>
+      <c r="K21" s="19">
+        <v>-0.29526172657404681</v>
+      </c>
+      <c r="L21" s="19">
+        <v>0.26690125229506823</v>
+      </c>
+      <c r="M21" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>n</v>
+      </c>
+      <c r="N21" s="33" t="str">
+        <f>IF(ISBLANK(I21),"",LOOKUP(ABS(I21),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
+        <v>None</v>
+      </c>
+      <c r="O21" s="33" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P21" s="20" t="str">
+        <f>IF(ABS(I21)&gt;ABS(all_tools!I21),"y","")</f>
+        <v/>
+      </c>
+      <c r="Q21" s="20" t="str">
+        <f>IF(ABS(I21)&lt;ABS(all_tools!I21),"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="R21" s="20" t="str">
+        <f>IF(M21=all_tools!M21,"y","")</f>
+        <v>y</v>
+      </c>
+      <c r="S21" s="61">
+        <f>ABS(I21)-ABS(all_tools!I21)</f>
+        <v>-3.5255674143355203E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="J23" t="s">
+        <v>50</v>
+      </c>
+      <c r="M23" s="3">
+        <f>M24-COUNTBLANK(M2:M21)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="J24" t="s">
+        <v>51</v>
+      </c>
+      <c r="M24" s="3">
+        <f>COUNTA(M2:M21)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="J25" t="s">
+        <v>46</v>
+      </c>
+      <c r="M25" s="3">
+        <f>COUNTIF(M2:M21,"y")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="J26" t="s">
+        <v>47</v>
+      </c>
+      <c r="M26" s="38">
+        <f>M25/M24</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="J27" t="s">
+        <v>48</v>
+      </c>
+      <c r="M27" s="3">
+        <f>M25-COUNTIFS(M2:M21,"y",N2:N21,"None")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="J28" t="s">
+        <v>49</v>
+      </c>
+      <c r="M28" s="38">
+        <f>M27/M24</f>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="J29" t="s">
+        <v>52</v>
+      </c>
+      <c r="M29" s="3">
+        <f>COUNTIF(N2:N21,"Medium")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="J30" t="s">
+        <v>53</v>
+      </c>
+      <c r="M30" s="38">
+        <f>M29/M24</f>
+        <v>0.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:O21" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O21">
+      <sortCondition ref="B1:B21"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="S20" activeCellId="8" sqref="S2 S3 S4 S9 S13 S17 S18 S19 S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2534,11 +3838,11 @@
       </c>
       <c r="P9" s="11" t="str">
         <f>IF(ABS(I9)&gt;ABS(all_tools!I9),"y","")</f>
-        <v/>
+        <v>y</v>
       </c>
       <c r="Q9" s="13" t="str">
         <f>IF(ABS(I9)&lt;ABS(all_tools!I9),"y","")</f>
-        <v>y</v>
+        <v/>
       </c>
       <c r="R9" s="13" t="str">
         <f>IF(M9=all_tools!M9,"y","")</f>
@@ -2546,7 +3850,7 @@
       </c>
       <c r="S9" s="47">
         <f>ABS(I9)-ABS(all_tools!I9)</f>
-        <v>-1.8914214859890699E-2</v>
+        <v>6.0911074785313601E-2</v>
       </c>
     </row>
     <row r="10" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -3423,12 +4727,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:S21"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3509,7 +4814,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -3575,7 +4880,7 @@
         <v>-0.16694523497703209</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
@@ -3641,7 +4946,7 @@
         <v>-0.21197556354848721</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
@@ -3707,7 +5012,7 @@
         <v>-0.22899208501055679</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>15</v>
       </c>
@@ -3769,7 +5074,7 @@
         <v>-0.20199933786647528</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
@@ -3958,7 +5263,7 @@
         <v>0.12053224189426359</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" s="11" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>19</v>
       </c>
@@ -4021,10 +5326,10 @@
       </c>
       <c r="S9" s="47">
         <f>ABS(I9)-ABS(all_tools!I9)</f>
-        <v>-9.1567000033513507E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.2">
+        <v>-1.1741710388309207E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>21</v>
       </c>
@@ -4090,7 +5395,7 @@
         <v>-3.9754675502425198E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>20</v>
       </c>
@@ -4222,7 +5527,7 @@
         <v>3.7275889888767899E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>22</v>
       </c>
@@ -4486,7 +5791,7 @@
         <v>-0.13127875321418006</v>
       </c>
     </row>
-    <row r="17" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
         <v>27</v>
       </c>
@@ -4552,7 +5857,7 @@
         <v>-9.6017443562945504E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
         <v>17</v>
       </c>
@@ -4618,7 +5923,7 @@
         <v>-9.6017443562945504E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>28</v>
       </c>
@@ -4684,7 +5989,7 @@
         <v>-1.3536763324230705E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
         <v>26</v>
       </c>
@@ -4750,7 +6055,7 @@
         <v>0.33308815162279104</v>
       </c>
     </row>
-    <row r="21" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" s="19" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>18</v>
       </c>
@@ -4890,6 +6195,16 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:O21" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <filterColumn colId="12">
+      <filters>
+        <filter val="n"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="13">
+      <filters>
+        <filter val="Small"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O21">
       <sortCondition ref="B1:B21"/>
     </sortState>
@@ -4898,7 +6213,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S30"/>
   <sheetViews>
@@ -5984,7 +7299,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S30"/>
   <sheetViews>

</xml_diff>